<commit_message>
added new green line excel
</commit_message>
<xml_diff>
--- a/src/CTC/Green_Line_ScheduleV2.xlsx
+++ b/src/CTC/Green_Line_ScheduleV2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\TrainsRepo\ECE1140ChooChoo\src\CTC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\ECE1140ChooChoo\src\CTC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4846726D-63F1-441C-B318-D3B00BFA5007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BC9A36C-8D89-4422-B1D3-DB7D74FDA316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3975" yWindow="6765" windowWidth="21600" windowHeight="11385" xr2:uid="{8B69A80D-850F-4154-9BF4-2347FAC8C2C8}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="22890" windowHeight="13980" xr2:uid="{8B69A80D-850F-4154-9BF4-2347FAC8C2C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -103,7 +103,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -136,7 +136,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,7 +474,7 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>